<commit_message>
Update Epicas y Historias de usuario.xlsx
</commit_message>
<xml_diff>
--- a/Fase 2/Evidencias Proyecto/Evidencias de documentación/Epicas y Historias de usuario.xlsx
+++ b/Fase 2/Evidencias Proyecto/Evidencias de documentación/Epicas y Historias de usuario.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC_211\Documents\GitHub\2024_2_PO_CAPSTONE_001D_GRUPO_2\Fase 2\Evidencias Proyecto\Evidencias de documentación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\devia\Desktop\2024_2_PO_CAPSTONE_001D_GRUPO_2\Fase 2\Evidencias Proyecto\Evidencias de documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4756F70D-9088-4941-B976-64CB1030A282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E706556B-B70D-4407-B268-AA7972AF328C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Epicas" sheetId="3" r:id="rId1"/>
@@ -289,7 +289,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -322,12 +322,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF4F4F4"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -335,6 +329,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFEEEEEE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -367,7 +391,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -394,32 +418,44 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -763,19 +799,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B71CC772-1B7D-4F8C-A429-9CC64CFA1080}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
     <col min="2" max="2" width="31.5" customWidth="1"/>
-    <col min="3" max="3" width="47.25" customWidth="1"/>
-    <col min="4" max="4" width="42.875" customWidth="1"/>
+    <col min="3" max="3" width="47.19921875" customWidth="1"/>
+    <col min="4" max="4" width="42.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="28.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -783,87 +819,87 @@
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="108" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
+    <row r="3" spans="1:4" ht="105.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="18">
         <v>1</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
+    <row r="4" spans="1:4" ht="92.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="19">
         <v>2</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="121.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="10">
+    <row r="5" spans="1:4" ht="132" x14ac:dyDescent="0.3">
+      <c r="A5" s="20">
         <v>3</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
+    <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="21">
         <v>4</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="121.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="10">
+    <row r="7" spans="1:4" ht="118.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="22">
         <v>5</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="12" t="s">
         <v>21</v>
       </c>
     </row>
@@ -880,28 +916,28 @@
   </sheetPr>
   <dimension ref="A1:M66"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.25" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26.875" customWidth="1"/>
-    <col min="3" max="3" width="24.25" customWidth="1"/>
-    <col min="4" max="5" width="48.75" customWidth="1"/>
-    <col min="6" max="6" width="3.25" customWidth="1"/>
+    <col min="1" max="1" width="3.19921875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.8984375" customWidth="1"/>
+    <col min="3" max="3" width="24.19921875" customWidth="1"/>
+    <col min="4" max="5" width="48.69921875" customWidth="1"/>
+    <col min="6" max="6" width="3.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
@@ -923,17 +959,17 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:13" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="10" t="s">
+    <row r="3" spans="1:13" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="12" t="s">
         <v>23</v>
       </c>
       <c r="F3" s="1"/>
@@ -945,17 +981,17 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:13" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="10" t="s">
+    <row r="4" spans="1:13" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="17" t="s">
         <v>25</v>
       </c>
       <c r="F4" s="1"/>
@@ -967,17 +1003,17 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:13" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="10" t="s">
+    <row r="5" spans="1:13" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="12" t="s">
         <v>27</v>
       </c>
       <c r="F5" s="1"/>
@@ -989,17 +1025,17 @@
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:13" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="10" t="s">
+    <row r="6" spans="1:13" ht="51" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="12" t="s">
         <v>29</v>
       </c>
       <c r="F6" s="1"/>
@@ -1011,17 +1047,17 @@
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
     </row>
-    <row r="7" spans="1:13" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="10" t="s">
+    <row r="7" spans="1:13" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="12" t="s">
         <v>31</v>
       </c>
       <c r="F7" s="1"/>
@@ -1033,17 +1069,17 @@
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="10" t="s">
+    <row r="8" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="12" t="s">
         <v>38</v>
       </c>
       <c r="F8" s="1"/>
@@ -1055,17 +1091,17 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="1:13" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="10" t="s">
+    <row r="9" spans="1:13" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="12" t="s">
         <v>40</v>
       </c>
       <c r="F9" s="1"/>
@@ -1077,17 +1113,17 @@
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
     </row>
-    <row r="10" spans="1:13" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="10" t="s">
+    <row r="10" spans="1:13" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="12" t="s">
         <v>44</v>
       </c>
       <c r="F10" s="1"/>
@@ -1099,17 +1135,17 @@
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
     </row>
-    <row r="11" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="10" t="s">
+    <row r="11" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="12" t="s">
         <v>46</v>
       </c>
       <c r="F11" s="1"/>
@@ -1121,17 +1157,17 @@
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
     </row>
-    <row r="12" spans="1:13" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="10" t="s">
+    <row r="12" spans="1:13" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E12" s="12" t="s">
         <v>50</v>
       </c>
       <c r="F12" s="1"/>
@@ -1143,17 +1179,17 @@
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
     </row>
-    <row r="13" spans="1:13" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="10" t="s">
+    <row r="13" spans="1:13" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="12" t="s">
         <v>52</v>
       </c>
       <c r="F13" s="1"/>
@@ -1165,17 +1201,17 @@
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
     </row>
-    <row r="14" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="10" t="s">
+    <row r="14" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="12" t="s">
         <v>54</v>
       </c>
       <c r="F14" s="1"/>
@@ -1187,17 +1223,17 @@
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
     </row>
-    <row r="15" spans="1:13" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="10" t="s">
+    <row r="15" spans="1:13" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="E15" s="12" t="s">
         <v>58</v>
       </c>
       <c r="F15" s="1"/>
@@ -1209,17 +1245,17 @@
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
     </row>
-    <row r="16" spans="1:13" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="10" t="s">
+    <row r="16" spans="1:13" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="12" t="s">
         <v>60</v>
       </c>
       <c r="F16" s="1"/>
@@ -1231,7 +1267,7 @@
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
     </row>
-    <row r="17" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -1245,7 +1281,7 @@
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -1259,7 +1295,7 @@
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
     </row>
-    <row r="19" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -1273,7 +1309,7 @@
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
     </row>
-    <row r="20" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -1287,7 +1323,7 @@
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
     </row>
-    <row r="21" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -1301,7 +1337,7 @@
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
     </row>
-    <row r="22" spans="2:13" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:13" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -1315,13 +1351,13 @@
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
     </row>
-    <row r="23" spans="2:13" s="9" customFormat="1" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:13" s="9" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -1335,7 +1371,7 @@
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -1349,7 +1385,7 @@
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -1363,7 +1399,7 @@
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -1377,7 +1413,7 @@
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -1391,7 +1427,7 @@
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -1405,7 +1441,7 @@
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -1419,7 +1455,7 @@
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -1433,7 +1469,7 @@
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -1447,7 +1483,7 @@
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -1461,7 +1497,7 @@
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -1475,7 +1511,7 @@
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -1489,7 +1525,7 @@
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
     </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -1503,7 +1539,7 @@
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
     </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -1517,7 +1553,7 @@
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
     </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -1531,7 +1567,7 @@
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
     </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
@@ -1545,7 +1581,7 @@
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
     </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
@@ -1559,7 +1595,7 @@
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
     </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
@@ -1573,7 +1609,7 @@
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
     </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
@@ -1587,7 +1623,7 @@
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
     </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -1601,7 +1637,7 @@
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
     </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -1615,7 +1651,7 @@
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
     </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
@@ -1629,7 +1665,7 @@
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
     </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -1643,7 +1679,7 @@
       <c r="L46" s="1"/>
       <c r="M46" s="1"/>
     </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -1657,7 +1693,7 @@
       <c r="L47" s="1"/>
       <c r="M47" s="1"/>
     </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
@@ -1671,7 +1707,7 @@
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
     </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
@@ -1685,7 +1721,7 @@
       <c r="L49" s="1"/>
       <c r="M49" s="1"/>
     </row>
-    <row r="50" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -1699,7 +1735,7 @@
       <c r="L50" s="1"/>
       <c r="M50" s="1"/>
     </row>
-    <row r="51" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -1713,7 +1749,7 @@
       <c r="L51" s="1"/>
       <c r="M51" s="1"/>
     </row>
-    <row r="52" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
@@ -1727,7 +1763,7 @@
       <c r="L52" s="1"/>
       <c r="M52" s="1"/>
     </row>
-    <row r="53" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -1741,7 +1777,7 @@
       <c r="L53" s="1"/>
       <c r="M53" s="1"/>
     </row>
-    <row r="54" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
@@ -1755,7 +1791,7 @@
       <c r="L54" s="1"/>
       <c r="M54" s="1"/>
     </row>
-    <row r="55" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
@@ -1769,7 +1805,7 @@
       <c r="L55" s="1"/>
       <c r="M55" s="1"/>
     </row>
-    <row r="56" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
@@ -1783,7 +1819,7 @@
       <c r="L56" s="1"/>
       <c r="M56" s="1"/>
     </row>
-    <row r="57" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
@@ -1797,7 +1833,7 @@
       <c r="L57" s="1"/>
       <c r="M57" s="1"/>
     </row>
-    <row r="58" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
@@ -1811,7 +1847,7 @@
       <c r="L58" s="1"/>
       <c r="M58" s="1"/>
     </row>
-    <row r="59" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
@@ -1825,7 +1861,7 @@
       <c r="L59" s="1"/>
       <c r="M59" s="1"/>
     </row>
-    <row r="60" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
@@ -1839,7 +1875,7 @@
       <c r="L60" s="1"/>
       <c r="M60" s="1"/>
     </row>
-    <row r="61" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
@@ -1853,7 +1889,7 @@
       <c r="L61" s="1"/>
       <c r="M61" s="1"/>
     </row>
-    <row r="62" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
@@ -1867,7 +1903,7 @@
       <c r="L62" s="1"/>
       <c r="M62" s="1"/>
     </row>
-    <row r="63" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
@@ -1881,7 +1917,7 @@
       <c r="L63" s="1"/>
       <c r="M63" s="1"/>
     </row>
-    <row r="64" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
@@ -1895,7 +1931,7 @@
       <c r="L64" s="1"/>
       <c r="M64" s="1"/>
     </row>
-    <row r="65" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
@@ -1909,7 +1945,7 @@
       <c r="L65" s="1"/>
       <c r="M65" s="1"/>
     </row>
-    <row r="66" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:13" x14ac:dyDescent="0.3">
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>

</xml_diff>